<commit_message>
implemented issuer bank accounts with client-side form and migration
</commit_message>
<xml_diff>
--- a/marer/templates/documents/issue_application_doc.xlsx
+++ b/marer/templates/documents/issue_application_doc.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="456">
   <si>
     <t>Аванс+</t>
   </si>
@@ -1847,6 +1847,18 @@
   </si>
   <si>
     <t>{issue.beneficiary_owner_4.on_belong_to_pub_persons_info}</t>
+  </si>
+  <si>
+    <t>{issue.bank_account_1.name}</t>
+  </si>
+  <si>
+    <t>{issue.bank_account_1.bik}</t>
+  </si>
+  <si>
+    <t>{issue.bank_account_2.name}</t>
+  </si>
+  <si>
+    <t>{issue.bank_account_2.bik}</t>
   </si>
 </sst>
 </file>
@@ -5569,7 +5581,7 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:ED265"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="A164" sqref="A164:BC164"/>
     </sheetView>
   </sheetViews>
@@ -10339,7 +10351,7 @@
       <c r="CB54" s="137"/>
       <c r="CC54" s="137"/>
     </row>
-    <row r="55" spans="1:81" ht="12" customHeight="1" outlineLevel="1">
+    <row r="55" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A55" s="311"/>
       <c r="B55" s="359"/>
       <c r="C55" s="359"/>
@@ -10422,7 +10434,7 @@
       <c r="CB55" s="137"/>
       <c r="CC55" s="137"/>
     </row>
-    <row r="56" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="56" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A56" s="368"/>
       <c r="B56" s="369"/>
       <c r="C56" s="369"/>
@@ -10505,7 +10517,7 @@
       <c r="CB56" s="137"/>
       <c r="CC56" s="137"/>
     </row>
-    <row r="57" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="57" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A57" s="361" t="s">
         <v>89</v>
       </c>
@@ -10590,7 +10602,7 @@
       <c r="CB57" s="137"/>
       <c r="CC57" s="137"/>
     </row>
-    <row r="58" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="58" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A58" s="364" t="s">
         <v>88</v>
       </c>
@@ -10675,7 +10687,7 @@
       <c r="CB58" s="137"/>
       <c r="CC58" s="137"/>
     </row>
-    <row r="59" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="59" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A59" s="319" t="s">
         <v>87</v>
       </c>
@@ -10760,7 +10772,7 @@
       <c r="CB59" s="137"/>
       <c r="CC59" s="137"/>
     </row>
-    <row r="60" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="60" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A60" s="325" t="s">
         <v>86</v>
       </c>
@@ -10845,7 +10857,7 @@
       <c r="CB60" s="137"/>
       <c r="CC60" s="137"/>
     </row>
-    <row r="61" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="61" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A61" s="329"/>
       <c r="B61" s="330"/>
       <c r="C61" s="330"/>
@@ -10928,7 +10940,7 @@
       <c r="CB61" s="137"/>
       <c r="CC61" s="137"/>
     </row>
-    <row r="62" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="62" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A62" s="338" t="s">
         <v>85</v>
       </c>
@@ -11015,7 +11027,7 @@
       <c r="CB62" s="137"/>
       <c r="CC62" s="137"/>
     </row>
-    <row r="63" spans="1:81" ht="13.5" customHeight="1" outlineLevel="3">
+    <row r="63" spans="1:81" ht="13.5" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A63" s="341"/>
       <c r="B63" s="342"/>
       <c r="C63" s="342"/>
@@ -11098,7 +11110,7 @@
       <c r="CB63" s="137"/>
       <c r="CC63" s="137"/>
     </row>
-    <row r="64" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="64" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A64" s="361" t="s">
         <v>89</v>
       </c>
@@ -11183,7 +11195,7 @@
       <c r="CB64" s="137"/>
       <c r="CC64" s="137"/>
     </row>
-    <row r="65" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="65" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A65" s="364" t="s">
         <v>88</v>
       </c>
@@ -11268,7 +11280,7 @@
       <c r="CB65" s="137"/>
       <c r="CC65" s="137"/>
     </row>
-    <row r="66" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="66" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A66" s="319" t="s">
         <v>87</v>
       </c>
@@ -11353,7 +11365,7 @@
       <c r="CB66" s="137"/>
       <c r="CC66" s="137"/>
     </row>
-    <row r="67" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="67" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A67" s="325" t="s">
         <v>86</v>
       </c>
@@ -11438,7 +11450,7 @@
       <c r="CB67" s="137"/>
       <c r="CC67" s="137"/>
     </row>
-    <row r="68" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="68" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A68" s="329"/>
       <c r="B68" s="330"/>
       <c r="C68" s="330"/>
@@ -11521,7 +11533,7 @@
       <c r="CB68" s="137"/>
       <c r="CC68" s="137"/>
     </row>
-    <row r="69" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="69" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A69" s="338" t="s">
         <v>85</v>
       </c>
@@ -11608,7 +11620,7 @@
       <c r="CB69" s="137"/>
       <c r="CC69" s="137"/>
     </row>
-    <row r="70" spans="1:81" ht="12.75" customHeight="1" outlineLevel="3">
+    <row r="70" spans="1:81" ht="12.75" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A70" s="341"/>
       <c r="B70" s="342"/>
       <c r="C70" s="342"/>
@@ -11691,7 +11703,7 @@
       <c r="CB70" s="137"/>
       <c r="CC70" s="137"/>
     </row>
-    <row r="71" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="71" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A71" s="361" t="s">
         <v>89</v>
       </c>
@@ -11776,7 +11788,7 @@
       <c r="CB71" s="137"/>
       <c r="CC71" s="137"/>
     </row>
-    <row r="72" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="72" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A72" s="364" t="s">
         <v>88</v>
       </c>
@@ -11861,7 +11873,7 @@
       <c r="CB72" s="137"/>
       <c r="CC72" s="137"/>
     </row>
-    <row r="73" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="73" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A73" s="319" t="s">
         <v>87</v>
       </c>
@@ -11946,7 +11958,7 @@
       <c r="CB73" s="137"/>
       <c r="CC73" s="137"/>
     </row>
-    <row r="74" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="74" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A74" s="325" t="s">
         <v>86</v>
       </c>
@@ -12031,7 +12043,7 @@
       <c r="CB74" s="137"/>
       <c r="CC74" s="137"/>
     </row>
-    <row r="75" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="75" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A75" s="329"/>
       <c r="B75" s="330"/>
       <c r="C75" s="330"/>
@@ -12114,7 +12126,7 @@
       <c r="CB75" s="137"/>
       <c r="CC75" s="137"/>
     </row>
-    <row r="76" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="76" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A76" s="338" t="s">
         <v>85</v>
       </c>
@@ -12201,7 +12213,7 @@
       <c r="CB76" s="137"/>
       <c r="CC76" s="137"/>
     </row>
-    <row r="77" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="77" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A77" s="341"/>
       <c r="B77" s="342"/>
       <c r="C77" s="342"/>
@@ -12284,7 +12296,7 @@
       <c r="CB77" s="137"/>
       <c r="CC77" s="137"/>
     </row>
-    <row r="78" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="78" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A78" s="361" t="s">
         <v>89</v>
       </c>
@@ -12369,7 +12381,7 @@
       <c r="CB78" s="137"/>
       <c r="CC78" s="137"/>
     </row>
-    <row r="79" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="79" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A79" s="364" t="s">
         <v>88</v>
       </c>
@@ -12454,7 +12466,7 @@
       <c r="CB79" s="137"/>
       <c r="CC79" s="137"/>
     </row>
-    <row r="80" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="80" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A80" s="319" t="s">
         <v>87</v>
       </c>
@@ -12539,7 +12551,7 @@
       <c r="CB80" s="137"/>
       <c r="CC80" s="137"/>
     </row>
-    <row r="81" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="81" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A81" s="325" t="s">
         <v>86</v>
       </c>
@@ -12624,7 +12636,7 @@
       <c r="CB81" s="137"/>
       <c r="CC81" s="137"/>
     </row>
-    <row r="82" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="82" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A82" s="329"/>
       <c r="B82" s="330"/>
       <c r="C82" s="330"/>
@@ -12707,7 +12719,7 @@
       <c r="CB82" s="137"/>
       <c r="CC82" s="137"/>
     </row>
-    <row r="83" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="83" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A83" s="338" t="s">
         <v>85</v>
       </c>
@@ -12794,7 +12806,7 @@
       <c r="CB83" s="137"/>
       <c r="CC83" s="137"/>
     </row>
-    <row r="84" spans="1:81" ht="12" customHeight="1" outlineLevel="3" collapsed="1">
+    <row r="84" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3" collapsed="1">
       <c r="A84" s="341"/>
       <c r="B84" s="342"/>
       <c r="C84" s="342"/>
@@ -12877,7 +12889,7 @@
       <c r="CB84" s="137"/>
       <c r="CC84" s="137"/>
     </row>
-    <row r="85" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="85" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A85" s="358"/>
       <c r="B85" s="371"/>
       <c r="C85" s="371"/>
@@ -12960,7 +12972,7 @@
       <c r="CB85" s="137"/>
       <c r="CC85" s="137"/>
     </row>
-    <row r="86" spans="1:81" ht="12" customHeight="1" outlineLevel="1">
+    <row r="86" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A86" s="368"/>
       <c r="B86" s="369"/>
       <c r="C86" s="369"/>
@@ -13043,7 +13055,7 @@
       <c r="CB86" s="137"/>
       <c r="CC86" s="137"/>
     </row>
-    <row r="87" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="87" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A87" s="361" t="s">
         <v>89</v>
       </c>
@@ -13128,7 +13140,7 @@
       <c r="CB87" s="137"/>
       <c r="CC87" s="137"/>
     </row>
-    <row r="88" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="88" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A88" s="364" t="s">
         <v>88</v>
       </c>
@@ -13213,7 +13225,7 @@
       <c r="CB88" s="137"/>
       <c r="CC88" s="137"/>
     </row>
-    <row r="89" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="89" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A89" s="319" t="s">
         <v>87</v>
       </c>
@@ -13298,7 +13310,7 @@
       <c r="CB89" s="137"/>
       <c r="CC89" s="137"/>
     </row>
-    <row r="90" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="90" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A90" s="325" t="s">
         <v>86</v>
       </c>
@@ -13383,7 +13395,7 @@
       <c r="CB90" s="137"/>
       <c r="CC90" s="137"/>
     </row>
-    <row r="91" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="91" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A91" s="329"/>
       <c r="B91" s="330"/>
       <c r="C91" s="330"/>
@@ -13466,7 +13478,7 @@
       <c r="CB91" s="137"/>
       <c r="CC91" s="137"/>
     </row>
-    <row r="92" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="92" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A92" s="338" t="s">
         <v>85</v>
       </c>
@@ -13553,7 +13565,7 @@
       <c r="CB92" s="137"/>
       <c r="CC92" s="137"/>
     </row>
-    <row r="93" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="93" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A93" s="341"/>
       <c r="B93" s="342"/>
       <c r="C93" s="342"/>
@@ -13636,7 +13648,7 @@
       <c r="CB93" s="137"/>
       <c r="CC93" s="137"/>
     </row>
-    <row r="94" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="94" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A94" s="361" t="s">
         <v>89</v>
       </c>
@@ -13721,7 +13733,7 @@
       <c r="CB94" s="137"/>
       <c r="CC94" s="137"/>
     </row>
-    <row r="95" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="95" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A95" s="364" t="s">
         <v>88</v>
       </c>
@@ -13806,7 +13818,7 @@
       <c r="CB95" s="137"/>
       <c r="CC95" s="137"/>
     </row>
-    <row r="96" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="96" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A96" s="319" t="s">
         <v>87</v>
       </c>
@@ -13891,7 +13903,7 @@
       <c r="CB96" s="137"/>
       <c r="CC96" s="137"/>
     </row>
-    <row r="97" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="97" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A97" s="325" t="s">
         <v>86</v>
       </c>
@@ -13976,7 +13988,7 @@
       <c r="CB97" s="137"/>
       <c r="CC97" s="137"/>
     </row>
-    <row r="98" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="98" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A98" s="329"/>
       <c r="B98" s="330"/>
       <c r="C98" s="330"/>
@@ -14059,7 +14071,7 @@
       <c r="CB98" s="137"/>
       <c r="CC98" s="137"/>
     </row>
-    <row r="99" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="99" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A99" s="338" t="s">
         <v>85</v>
       </c>
@@ -14146,7 +14158,7 @@
       <c r="CB99" s="137"/>
       <c r="CC99" s="137"/>
     </row>
-    <row r="100" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="100" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A100" s="341"/>
       <c r="B100" s="342"/>
       <c r="C100" s="342"/>
@@ -14229,7 +14241,7 @@
       <c r="CB100" s="137"/>
       <c r="CC100" s="137"/>
     </row>
-    <row r="101" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="101" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A101" s="361" t="s">
         <v>89</v>
       </c>
@@ -14314,7 +14326,7 @@
       <c r="CB101" s="137"/>
       <c r="CC101" s="137"/>
     </row>
-    <row r="102" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="102" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A102" s="364" t="s">
         <v>88</v>
       </c>
@@ -14399,7 +14411,7 @@
       <c r="CB102" s="137"/>
       <c r="CC102" s="137"/>
     </row>
-    <row r="103" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="103" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A103" s="319" t="s">
         <v>87</v>
       </c>
@@ -14484,7 +14496,7 @@
       <c r="CB103" s="137"/>
       <c r="CC103" s="137"/>
     </row>
-    <row r="104" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="104" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A104" s="325" t="s">
         <v>86</v>
       </c>
@@ -14569,7 +14581,7 @@
       <c r="CB104" s="137"/>
       <c r="CC104" s="137"/>
     </row>
-    <row r="105" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="105" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A105" s="329"/>
       <c r="B105" s="330"/>
       <c r="C105" s="330"/>
@@ -14652,7 +14664,7 @@
       <c r="CB105" s="137"/>
       <c r="CC105" s="137"/>
     </row>
-    <row r="106" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="106" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A106" s="338" t="s">
         <v>85</v>
       </c>
@@ -14739,7 +14751,7 @@
       <c r="CB106" s="137"/>
       <c r="CC106" s="137"/>
     </row>
-    <row r="107" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="107" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A107" s="341"/>
       <c r="B107" s="342"/>
       <c r="C107" s="342"/>
@@ -14822,7 +14834,7 @@
       <c r="CB107" s="137"/>
       <c r="CC107" s="137"/>
     </row>
-    <row r="108" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="108" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A108" s="361" t="s">
         <v>89</v>
       </c>
@@ -14907,7 +14919,7 @@
       <c r="CB108" s="137"/>
       <c r="CC108" s="137"/>
     </row>
-    <row r="109" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="109" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A109" s="364" t="s">
         <v>88</v>
       </c>
@@ -14992,7 +15004,7 @@
       <c r="CB109" s="137"/>
       <c r="CC109" s="137"/>
     </row>
-    <row r="110" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="110" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A110" s="319" t="s">
         <v>87</v>
       </c>
@@ -15077,7 +15089,7 @@
       <c r="CB110" s="137"/>
       <c r="CC110" s="137"/>
     </row>
-    <row r="111" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="111" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A111" s="325" t="s">
         <v>86</v>
       </c>
@@ -15162,7 +15174,7 @@
       <c r="CB111" s="137"/>
       <c r="CC111" s="137"/>
     </row>
-    <row r="112" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="112" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A112" s="329"/>
       <c r="B112" s="330"/>
       <c r="C112" s="330"/>
@@ -15245,7 +15257,7 @@
       <c r="CB112" s="137"/>
       <c r="CC112" s="137"/>
     </row>
-    <row r="113" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="113" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A113" s="338" t="s">
         <v>85</v>
       </c>
@@ -15332,7 +15344,7 @@
       <c r="CB113" s="137"/>
       <c r="CC113" s="137"/>
     </row>
-    <row r="114" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="114" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A114" s="341"/>
       <c r="B114" s="342"/>
       <c r="C114" s="342"/>
@@ -15415,7 +15427,7 @@
       <c r="CB114" s="137"/>
       <c r="CC114" s="137"/>
     </row>
-    <row r="115" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="115" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A115" s="361" t="s">
         <v>89</v>
       </c>
@@ -15500,7 +15512,7 @@
       <c r="CB115" s="137"/>
       <c r="CC115" s="137"/>
     </row>
-    <row r="116" spans="1:81" ht="12" customHeight="1" outlineLevel="4">
+    <row r="116" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="4">
       <c r="A116" s="364" t="s">
         <v>88</v>
       </c>
@@ -15585,7 +15597,7 @@
       <c r="CB116" s="137"/>
       <c r="CC116" s="137"/>
     </row>
-    <row r="117" spans="1:81" ht="12" customHeight="1" outlineLevel="4">
+    <row r="117" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="4">
       <c r="A117" s="319" t="s">
         <v>87</v>
       </c>
@@ -15670,7 +15682,7 @@
       <c r="CB117" s="137"/>
       <c r="CC117" s="137"/>
     </row>
-    <row r="118" spans="1:81" ht="12" customHeight="1" outlineLevel="4">
+    <row r="118" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="4">
       <c r="A118" s="325" t="s">
         <v>86</v>
       </c>
@@ -15755,7 +15767,7 @@
       <c r="CB118" s="137"/>
       <c r="CC118" s="137"/>
     </row>
-    <row r="119" spans="1:81" ht="12" customHeight="1" outlineLevel="4">
+    <row r="119" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="4">
       <c r="A119" s="329"/>
       <c r="B119" s="330"/>
       <c r="C119" s="330"/>
@@ -15838,7 +15850,7 @@
       <c r="CB119" s="137"/>
       <c r="CC119" s="137"/>
     </row>
-    <row r="120" spans="1:81" ht="12" customHeight="1" outlineLevel="4">
+    <row r="120" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="4">
       <c r="A120" s="338" t="s">
         <v>85</v>
       </c>
@@ -15925,7 +15937,7 @@
       <c r="CB120" s="137"/>
       <c r="CC120" s="137"/>
     </row>
-    <row r="121" spans="1:81" ht="12" customHeight="1" outlineLevel="4">
+    <row r="121" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="4">
       <c r="A121" s="341"/>
       <c r="B121" s="342"/>
       <c r="C121" s="342"/>
@@ -16008,7 +16020,7 @@
       <c r="CB121" s="137"/>
       <c r="CC121" s="137"/>
     </row>
-    <row r="122" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="122" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A122" s="368"/>
       <c r="B122" s="369"/>
       <c r="C122" s="369"/>
@@ -16091,7 +16103,7 @@
       <c r="CB122" s="137"/>
       <c r="CC122" s="137"/>
     </row>
-    <row r="123" spans="1:81" ht="12" customHeight="1" outlineLevel="1">
+    <row r="123" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A123" s="368"/>
       <c r="B123" s="369"/>
       <c r="C123" s="369"/>
@@ -16174,7 +16186,7 @@
       <c r="CB123" s="137"/>
       <c r="CC123" s="137"/>
     </row>
-    <row r="124" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="124" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A124" s="361" t="s">
         <v>89</v>
       </c>
@@ -16259,7 +16271,7 @@
       <c r="CB124" s="137"/>
       <c r="CC124" s="137"/>
     </row>
-    <row r="125" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="125" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A125" s="364" t="s">
         <v>88</v>
       </c>
@@ -16344,7 +16356,7 @@
       <c r="CB125" s="137"/>
       <c r="CC125" s="137"/>
     </row>
-    <row r="126" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="126" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A126" s="319" t="s">
         <v>87</v>
       </c>
@@ -16429,7 +16441,7 @@
       <c r="CB126" s="137"/>
       <c r="CC126" s="137"/>
     </row>
-    <row r="127" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="127" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A127" s="325" t="s">
         <v>86</v>
       </c>
@@ -16514,7 +16526,7 @@
       <c r="CB127" s="137"/>
       <c r="CC127" s="137"/>
     </row>
-    <row r="128" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="128" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A128" s="329"/>
       <c r="B128" s="330"/>
       <c r="C128" s="330"/>
@@ -16597,7 +16609,7 @@
       <c r="CB128" s="137"/>
       <c r="CC128" s="137"/>
     </row>
-    <row r="129" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="129" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A129" s="338" t="s">
         <v>85</v>
       </c>
@@ -16684,7 +16696,7 @@
       <c r="CB129" s="137"/>
       <c r="CC129" s="137"/>
     </row>
-    <row r="130" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="130" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A130" s="341"/>
       <c r="B130" s="342"/>
       <c r="C130" s="342"/>
@@ -16767,7 +16779,7 @@
       <c r="CB130" s="137"/>
       <c r="CC130" s="137"/>
     </row>
-    <row r="131" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="131" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A131" s="361" t="s">
         <v>89</v>
       </c>
@@ -16852,7 +16864,7 @@
       <c r="CB131" s="137"/>
       <c r="CC131" s="137"/>
     </row>
-    <row r="132" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="132" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A132" s="364" t="s">
         <v>88</v>
       </c>
@@ -16937,7 +16949,7 @@
       <c r="CB132" s="137"/>
       <c r="CC132" s="137"/>
     </row>
-    <row r="133" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="133" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A133" s="319" t="s">
         <v>87</v>
       </c>
@@ -17022,7 +17034,7 @@
       <c r="CB133" s="137"/>
       <c r="CC133" s="137"/>
     </row>
-    <row r="134" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="134" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A134" s="325" t="s">
         <v>86</v>
       </c>
@@ -17107,7 +17119,7 @@
       <c r="CB134" s="137"/>
       <c r="CC134" s="137"/>
     </row>
-    <row r="135" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="135" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A135" s="329"/>
       <c r="B135" s="330"/>
       <c r="C135" s="330"/>
@@ -17190,7 +17202,7 @@
       <c r="CB135" s="137"/>
       <c r="CC135" s="137"/>
     </row>
-    <row r="136" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="136" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A136" s="338" t="s">
         <v>85</v>
       </c>
@@ -17277,7 +17289,7 @@
       <c r="CB136" s="137"/>
       <c r="CC136" s="137"/>
     </row>
-    <row r="137" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="137" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A137" s="341"/>
       <c r="B137" s="342"/>
       <c r="C137" s="342"/>
@@ -17360,7 +17372,7 @@
       <c r="CB137" s="137"/>
       <c r="CC137" s="137"/>
     </row>
-    <row r="138" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="138" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A138" s="361" t="s">
         <v>89</v>
       </c>
@@ -17445,7 +17457,7 @@
       <c r="CB138" s="137"/>
       <c r="CC138" s="137"/>
     </row>
-    <row r="139" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="139" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A139" s="364" t="s">
         <v>88</v>
       </c>
@@ -17530,7 +17542,7 @@
       <c r="CB139" s="137"/>
       <c r="CC139" s="137"/>
     </row>
-    <row r="140" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="140" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A140" s="319" t="s">
         <v>87</v>
       </c>
@@ -17615,7 +17627,7 @@
       <c r="CB140" s="137"/>
       <c r="CC140" s="137"/>
     </row>
-    <row r="141" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="141" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A141" s="325" t="s">
         <v>86</v>
       </c>
@@ -17700,7 +17712,7 @@
       <c r="CB141" s="137"/>
       <c r="CC141" s="137"/>
     </row>
-    <row r="142" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="142" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A142" s="329"/>
       <c r="B142" s="330"/>
       <c r="C142" s="330"/>
@@ -17783,7 +17795,7 @@
       <c r="CB142" s="137"/>
       <c r="CC142" s="137"/>
     </row>
-    <row r="143" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="143" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A143" s="338" t="s">
         <v>85</v>
       </c>
@@ -17870,7 +17882,7 @@
       <c r="CB143" s="137"/>
       <c r="CC143" s="137"/>
     </row>
-    <row r="144" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="144" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A144" s="341"/>
       <c r="B144" s="342"/>
       <c r="C144" s="342"/>
@@ -17953,7 +17965,7 @@
       <c r="CB144" s="137"/>
       <c r="CC144" s="137"/>
     </row>
-    <row r="145" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="145" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A145" s="361" t="s">
         <v>89</v>
       </c>
@@ -18038,7 +18050,7 @@
       <c r="CB145" s="137"/>
       <c r="CC145" s="137"/>
     </row>
-    <row r="146" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="146" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A146" s="364" t="s">
         <v>88</v>
       </c>
@@ -18123,7 +18135,7 @@
       <c r="CB146" s="137"/>
       <c r="CC146" s="137"/>
     </row>
-    <row r="147" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="147" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A147" s="319" t="s">
         <v>87</v>
       </c>
@@ -18208,7 +18220,7 @@
       <c r="CB147" s="137"/>
       <c r="CC147" s="137"/>
     </row>
-    <row r="148" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="148" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A148" s="325" t="s">
         <v>86</v>
       </c>
@@ -18293,7 +18305,7 @@
       <c r="CB148" s="137"/>
       <c r="CC148" s="137"/>
     </row>
-    <row r="149" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="149" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A149" s="329"/>
       <c r="B149" s="330"/>
       <c r="C149" s="330"/>
@@ -18376,7 +18388,7 @@
       <c r="CB149" s="137"/>
       <c r="CC149" s="137"/>
     </row>
-    <row r="150" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="150" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A150" s="338" t="s">
         <v>85</v>
       </c>
@@ -18463,7 +18475,7 @@
       <c r="CB150" s="137"/>
       <c r="CC150" s="137"/>
     </row>
-    <row r="151" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="151" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A151" s="341"/>
       <c r="B151" s="342"/>
       <c r="C151" s="342"/>
@@ -18546,7 +18558,7 @@
       <c r="CB151" s="137"/>
       <c r="CC151" s="137"/>
     </row>
-    <row r="152" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="152" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A152" s="361" t="s">
         <v>89</v>
       </c>
@@ -18631,7 +18643,7 @@
       <c r="CB152" s="137"/>
       <c r="CC152" s="137"/>
     </row>
-    <row r="153" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="153" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A153" s="364" t="s">
         <v>88</v>
       </c>
@@ -18716,7 +18728,7 @@
       <c r="CB153" s="137"/>
       <c r="CC153" s="137"/>
     </row>
-    <row r="154" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="154" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A154" s="319" t="s">
         <v>87</v>
       </c>
@@ -18801,7 +18813,7 @@
       <c r="CB154" s="137"/>
       <c r="CC154" s="137"/>
     </row>
-    <row r="155" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="155" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A155" s="325" t="s">
         <v>86</v>
       </c>
@@ -18886,7 +18898,7 @@
       <c r="CB155" s="137"/>
       <c r="CC155" s="137"/>
     </row>
-    <row r="156" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="156" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A156" s="329"/>
       <c r="B156" s="330"/>
       <c r="C156" s="330"/>
@@ -18969,7 +18981,7 @@
       <c r="CB156" s="137"/>
       <c r="CC156" s="137"/>
     </row>
-    <row r="157" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="157" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A157" s="338" t="s">
         <v>85</v>
       </c>
@@ -19056,7 +19068,7 @@
       <c r="CB157" s="137"/>
       <c r="CC157" s="137"/>
     </row>
-    <row r="158" spans="1:81" ht="12" customHeight="1" outlineLevel="3">
+    <row r="158" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="3">
       <c r="A158" s="341"/>
       <c r="B158" s="342"/>
       <c r="C158" s="342"/>
@@ -19139,7 +19151,7 @@
       <c r="CB158" s="137"/>
       <c r="CC158" s="137"/>
     </row>
-    <row r="159" spans="1:81" ht="12" customHeight="1" outlineLevel="2">
+    <row r="159" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="2">
       <c r="A159" s="358"/>
       <c r="B159" s="359"/>
       <c r="C159" s="359"/>
@@ -19222,7 +19234,7 @@
       <c r="CB159" s="137"/>
       <c r="CC159" s="137"/>
     </row>
-    <row r="160" spans="1:81" ht="12" customHeight="1" outlineLevel="1">
+    <row r="160" spans="1:81" ht="12" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A160" s="358"/>
       <c r="B160" s="359"/>
       <c r="C160" s="359"/>
@@ -19305,7 +19317,7 @@
       <c r="CB160" s="137"/>
       <c r="CC160" s="137"/>
     </row>
-    <row r="161" spans="1:81" ht="14.25" customHeight="1">
+    <row r="161" spans="1:81" ht="14.25" customHeight="1" collapsed="1">
       <c r="A161" s="319" t="s">
         <v>83</v>
       </c>
@@ -20520,7 +20532,9 @@
       <c r="CC174" s="137"/>
     </row>
     <row r="175" spans="1:81" ht="12.95" customHeight="1">
-      <c r="A175" s="394"/>
+      <c r="A175" s="394" t="s">
+        <v>452</v>
+      </c>
       <c r="B175" s="395"/>
       <c r="C175" s="395"/>
       <c r="D175" s="395"/>
@@ -20575,7 +20589,9 @@
       <c r="BA175" s="395"/>
       <c r="BB175" s="395"/>
       <c r="BC175" s="396"/>
-      <c r="BD175" s="394"/>
+      <c r="BD175" s="394" t="s">
+        <v>453</v>
+      </c>
       <c r="BE175" s="395"/>
       <c r="BF175" s="395"/>
       <c r="BG175" s="395"/>
@@ -20603,7 +20619,9 @@
       <c r="CC175" s="137"/>
     </row>
     <row r="176" spans="1:81" ht="12.95" customHeight="1">
-      <c r="A176" s="322"/>
+      <c r="A176" s="322" t="s">
+        <v>454</v>
+      </c>
       <c r="B176" s="379"/>
       <c r="C176" s="379"/>
       <c r="D176" s="379"/>
@@ -20658,7 +20676,9 @@
       <c r="BA176" s="379"/>
       <c r="BB176" s="379"/>
       <c r="BC176" s="380"/>
-      <c r="BD176" s="397"/>
+      <c r="BD176" s="397" t="s">
+        <v>455</v>
+      </c>
       <c r="BE176" s="398"/>
       <c r="BF176" s="398"/>
       <c r="BG176" s="398"/>
@@ -21624,7 +21644,7 @@
       <c r="CB187" s="137"/>
       <c r="CC187" s="137"/>
     </row>
-    <row r="188" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="188" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A188" s="319" t="s">
         <v>74</v>
       </c>
@@ -21711,7 +21731,7 @@
       <c r="CB188" s="137"/>
       <c r="CC188" s="137"/>
     </row>
-    <row r="189" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="189" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A189" s="319" t="s">
         <v>73</v>
       </c>
@@ -21798,7 +21818,7 @@
       <c r="CB189" s="137"/>
       <c r="CC189" s="137"/>
     </row>
-    <row r="190" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="190" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A190" s="319" t="s">
         <v>72</v>
       </c>
@@ -21885,7 +21905,7 @@
       <c r="CB190" s="137"/>
       <c r="CC190" s="137"/>
     </row>
-    <row r="191" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="191" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A191" s="319" t="s">
         <v>71</v>
       </c>
@@ -21972,7 +21992,7 @@
       <c r="CB191" s="137"/>
       <c r="CC191" s="137"/>
     </row>
-    <row r="192" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="192" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A192" s="319" t="s">
         <v>70</v>
       </c>
@@ -22059,7 +22079,7 @@
       <c r="CB192" s="137"/>
       <c r="CC192" s="137"/>
     </row>
-    <row r="193" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="193" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A193" s="338" t="s">
         <v>69</v>
       </c>
@@ -22146,7 +22166,7 @@
       <c r="CB193" s="137"/>
       <c r="CC193" s="137"/>
     </row>
-    <row r="194" spans="1:81" ht="11.25" customHeight="1" outlineLevel="1">
+    <row r="194" spans="1:81" ht="11.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A194" s="341"/>
       <c r="B194" s="342"/>
       <c r="C194" s="342"/>
@@ -22229,7 +22249,7 @@
       <c r="CB194" s="137"/>
       <c r="CC194" s="137"/>
     </row>
-    <row r="195" spans="1:81" ht="9" customHeight="1">
+    <row r="195" spans="1:81" ht="9" customHeight="1" collapsed="1">
       <c r="A195" s="144"/>
       <c r="B195" s="144"/>
       <c r="C195" s="144"/>
@@ -22312,7 +22332,7 @@
       <c r="CB195" s="137"/>
       <c r="CC195" s="137"/>
     </row>
-    <row r="196" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="196" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A196" s="319" t="s">
         <v>74</v>
       </c>
@@ -22399,7 +22419,7 @@
       <c r="CB196" s="137"/>
       <c r="CC196" s="137"/>
     </row>
-    <row r="197" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="197" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A197" s="319" t="s">
         <v>73</v>
       </c>
@@ -22486,7 +22506,7 @@
       <c r="CB197" s="137"/>
       <c r="CC197" s="137"/>
     </row>
-    <row r="198" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="198" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A198" s="319" t="s">
         <v>72</v>
       </c>
@@ -22573,7 +22593,7 @@
       <c r="CB198" s="137"/>
       <c r="CC198" s="137"/>
     </row>
-    <row r="199" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="199" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A199" s="319" t="s">
         <v>71</v>
       </c>
@@ -22660,7 +22680,7 @@
       <c r="CB199" s="137"/>
       <c r="CC199" s="137"/>
     </row>
-    <row r="200" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="200" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A200" s="319" t="s">
         <v>70</v>
       </c>
@@ -22747,7 +22767,7 @@
       <c r="CB200" s="137"/>
       <c r="CC200" s="137"/>
     </row>
-    <row r="201" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="201" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A201" s="338" t="s">
         <v>69</v>
       </c>
@@ -22834,7 +22854,7 @@
       <c r="CB201" s="137"/>
       <c r="CC201" s="137"/>
     </row>
-    <row r="202" spans="1:81" ht="11.25" customHeight="1" outlineLevel="1">
+    <row r="202" spans="1:81" ht="11.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A202" s="341"/>
       <c r="B202" s="342"/>
       <c r="C202" s="342"/>
@@ -22917,7 +22937,7 @@
       <c r="CB202" s="137"/>
       <c r="CC202" s="137"/>
     </row>
-    <row r="203" spans="1:81" ht="9" customHeight="1">
+    <row r="203" spans="1:81" ht="9" customHeight="1" collapsed="1">
       <c r="A203" s="144"/>
       <c r="B203" s="144"/>
       <c r="C203" s="144"/>
@@ -23000,7 +23020,7 @@
       <c r="CB203" s="137"/>
       <c r="CC203" s="137"/>
     </row>
-    <row r="204" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="204" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A204" s="319" t="s">
         <v>74</v>
       </c>
@@ -23087,7 +23107,7 @@
       <c r="CB204" s="137"/>
       <c r="CC204" s="137"/>
     </row>
-    <row r="205" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="205" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A205" s="319" t="s">
         <v>73</v>
       </c>
@@ -23174,7 +23194,7 @@
       <c r="CB205" s="137"/>
       <c r="CC205" s="137"/>
     </row>
-    <row r="206" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="206" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A206" s="319" t="s">
         <v>72</v>
       </c>
@@ -23261,7 +23281,7 @@
       <c r="CB206" s="137"/>
       <c r="CC206" s="137"/>
     </row>
-    <row r="207" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="207" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A207" s="319" t="s">
         <v>71</v>
       </c>
@@ -23348,7 +23368,7 @@
       <c r="CB207" s="137"/>
       <c r="CC207" s="137"/>
     </row>
-    <row r="208" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="208" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A208" s="319" t="s">
         <v>70</v>
       </c>
@@ -23435,7 +23455,7 @@
       <c r="CB208" s="137"/>
       <c r="CC208" s="137"/>
     </row>
-    <row r="209" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="209" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A209" s="338" t="s">
         <v>69</v>
       </c>
@@ -23522,7 +23542,7 @@
       <c r="CB209" s="137"/>
       <c r="CC209" s="137"/>
     </row>
-    <row r="210" spans="1:81" ht="12.95" customHeight="1" outlineLevel="1">
+    <row r="210" spans="1:81" ht="12.95" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A210" s="341"/>
       <c r="B210" s="342"/>
       <c r="C210" s="342"/>
@@ -23605,7 +23625,7 @@
       <c r="CB210" s="137"/>
       <c r="CC210" s="137"/>
     </row>
-    <row r="211" spans="1:81" ht="5.25" customHeight="1" outlineLevel="1">
+    <row r="211" spans="1:81" ht="5.25" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A211" s="311"/>
       <c r="B211" s="312"/>
       <c r="C211" s="312"/>
@@ -23688,7 +23708,7 @@
       <c r="CB211" s="137"/>
       <c r="CC211" s="137"/>
     </row>
-    <row r="212" spans="1:81" ht="13.5" customHeight="1">
+    <row r="212" spans="1:81" ht="13.5" customHeight="1" collapsed="1">
       <c r="A212" s="302" t="s">
         <v>168</v>
       </c>
@@ -36798,15 +36818,15 @@
       <c r="F2" s="184"/>
       <c r="H2" s="263">
         <f ca="1">NOW()</f>
-        <v>43090.504734722221</v>
+        <v>43090.551654050927</v>
       </c>
       <c r="I2" s="264">
         <f ca="1">H2</f>
-        <v>43090.504734722221</v>
+        <v>43090.551654050927</v>
       </c>
       <c r="J2" s="264">
         <f ca="1">MOD(I2,1)</f>
-        <v>0.50473472222074633</v>
+        <v>0.55165405092702713</v>
       </c>
       <c r="K2" s="265">
         <f ca="1">I2-J2</f>
@@ -36838,7 +36858,7 @@
       <c r="F3" s="184"/>
       <c r="J3" s="265">
         <f ca="1">INT(J2*100000)</f>
-        <v>50473</v>
+        <v>55165</v>
       </c>
       <c r="K3" s="265">
         <f ca="1">K2-42900</f>
@@ -36872,7 +36892,7 @@
       </c>
       <c r="J4" s="174" t="str">
         <f ca="1">L2&amp;K3&amp;-J3&amp;L3</f>
-        <v>19/190-50473ЭГ-17</v>
+        <v>19/190-55165ЭГ-17</v>
       </c>
     </row>
     <row r="5" spans="1:25" hidden="1" outlineLevel="1">
@@ -36909,11 +36929,11 @@
       </c>
       <c r="B6" s="182" t="str">
         <f ca="1">J4</f>
-        <v>19/190-50473ЭГ-17</v>
+        <v>19/190-55165ЭГ-17</v>
       </c>
       <c r="C6" s="186" t="str">
         <f ca="1">B6</f>
-        <v>19/190-50473ЭГ-17</v>
+        <v>19/190-55165ЭГ-17</v>
       </c>
       <c r="D6" s="183" t="s">
         <v>382</v>

</xml_diff>